<commit_message>
Adding test results to PolyBench 4.0
</commit_message>
<xml_diff>
--- a/tests/polybench-c-4.0/results/isl-checks-vs-newest-polly-restrict.xlsx
+++ b/tests/polybench-c-4.0/results/isl-checks-vs-newest-polly-restrict.xlsx
@@ -190,7 +190,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -199,15 +199,9 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
@@ -217,30 +211,15 @@
       <left style="medium">
         <color auto="1"/>
       </left>
-      <right style="medium">
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
+      <left/>
       <right style="medium">
         <color auto="1"/>
       </right>
@@ -250,6 +229,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -304,22 +301,6 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -328,6 +309,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -623,11 +620,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2099682744"/>
-        <c:axId val="2099685656"/>
+        <c:axId val="2110011528"/>
+        <c:axId val="2110014536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2099682744"/>
+        <c:axId val="2110011528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -636,7 +633,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099685656"/>
+        <c:crossAx val="2110014536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -644,7 +641,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2099685656"/>
+        <c:axId val="2110014536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.75"/>
@@ -666,7 +663,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099682744"/>
+        <c:crossAx val="2110011528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.25"/>
@@ -1170,128 +1167,127 @@
   <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:M5"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-    </row>
-    <row r="6" spans="1:17" ht="16" thickBot="1"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+    </row>
     <row r="7" spans="1:17" ht="16" thickBot="1">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="11">
         <v>1.33735E-2</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="12">
         <v>1.2482E-2</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="6">
         <f t="shared" ref="D8:D36" si="0">C8/B8</f>
         <v>0.93333831831607283</v>
       </c>
@@ -1300,10 +1296,10 @@
       <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="11">
         <v>0.94579283300000005</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="12">
         <v>0.90737016699999995</v>
       </c>
       <c r="D9" s="6">
@@ -1315,10 +1311,10 @@
       <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="11">
         <v>2.9314770000000001</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="12">
         <v>2.836864667</v>
       </c>
       <c r="D10" s="6">
@@ -1330,10 +1326,10 @@
       <c r="A11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="11">
         <v>9.2170433329999994</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="12">
         <v>9.0783044999999998</v>
       </c>
       <c r="D11" s="6">
@@ -1345,10 +1341,10 @@
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="11">
         <v>3.2021167000000003E-2</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="12">
         <v>3.1623499999999999E-2</v>
       </c>
       <c r="D12" s="6">
@@ -1360,10 +1356,10 @@
       <c r="A13" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="11">
         <v>1.9945167E-2</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="12">
         <v>1.9716833E-2</v>
       </c>
       <c r="D13" s="6">
@@ -1375,10 +1371,10 @@
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="11">
         <v>5.3946669999999997E-3</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="12">
         <v>5.3383329999999998E-3</v>
       </c>
       <c r="D14" s="6">
@@ -1390,10 +1386,10 @@
       <c r="A15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="11">
         <v>4.9403784999999996</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="12">
         <v>4.9002193329999999</v>
       </c>
       <c r="D15" s="6">
@@ -1405,10 +1401,10 @@
       <c r="A16" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="11">
         <v>2.0997221669999999</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="12">
         <v>2.0849031669999998</v>
       </c>
       <c r="D16" s="6">
@@ -1420,10 +1416,10 @@
       <c r="A17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="11">
         <v>1.6933640000000001</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="12">
         <v>1.6823859999999999</v>
       </c>
       <c r="D17" s="6">
@@ -1435,10 +1431,10 @@
       <c r="A18" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="11">
         <v>6.1111669999999998E-3</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="12">
         <v>6.0851669999999998E-3</v>
       </c>
       <c r="D18" s="6">
@@ -1450,10 +1446,10 @@
       <c r="A19" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="11">
         <v>31.796257669999999</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="12">
         <v>31.717261329999999</v>
       </c>
       <c r="D19" s="6">
@@ -1465,10 +1461,10 @@
       <c r="A20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="11">
         <v>23.106549999999999</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="12">
         <v>23.053478670000001</v>
       </c>
       <c r="D20" s="6">
@@ -1480,10 +1476,10 @@
       <c r="A21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="11">
         <v>1.773596333</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="12">
         <v>1.7725503330000001</v>
       </c>
       <c r="D21" s="6">
@@ -1495,10 +1491,10 @@
       <c r="A22" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="11">
         <v>1.282573333</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="12">
         <v>1.281836167</v>
       </c>
       <c r="D22" s="6">
@@ -1510,10 +1506,10 @@
       <c r="A23" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="11">
         <v>1.544563833</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="12">
         <v>1.5456413330000001</v>
       </c>
       <c r="D23" s="6">
@@ -1525,10 +1521,10 @@
       <c r="A24" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="11">
         <v>8.1919953329999995</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="12">
         <v>8.2647073330000005</v>
       </c>
       <c r="D24" s="6">
@@ -1540,10 +1536,10 @@
       <c r="A25" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="11">
         <v>1.2783948329999999</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="12">
         <v>1.2913714999999999</v>
       </c>
       <c r="D25" s="6">
@@ -1555,26 +1551,26 @@
       <c r="A26" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="11">
         <v>3.4664955000000002</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="12">
         <v>3.5026266669999999</v>
       </c>
       <c r="D26" s="6">
         <f t="shared" si="0"/>
         <v>1.0104229666532092</v>
       </c>
-      <c r="G26" s="9"/>
+      <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="11">
         <v>0.244437667</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="12">
         <v>0.247467833</v>
       </c>
       <c r="D27" s="6">
@@ -1586,10 +1582,10 @@
       <c r="A28" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="11">
         <v>1.9664999999999998E-2</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="12">
         <v>1.9987167E-2</v>
       </c>
       <c r="D28" s="6">
@@ -1601,10 +1597,10 @@
       <c r="A29" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="11">
         <v>3.3235026670000001</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="12">
         <v>3.3894700000000002</v>
       </c>
       <c r="D29" s="6">
@@ -1616,10 +1612,10 @@
       <c r="A30" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="11">
         <v>2.558214167</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="12">
         <v>2.6121371670000002</v>
       </c>
       <c r="D30" s="6">
@@ -1631,10 +1627,10 @@
       <c r="A31" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="11">
         <v>4.4038330000000002E-3</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="12">
         <v>4.5694999999999998E-3</v>
       </c>
       <c r="D31" s="6">
@@ -1646,10 +1642,10 @@
       <c r="A32" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="11">
         <v>0.52918316700000001</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="12">
         <v>0.58997299999999997</v>
       </c>
       <c r="D32" s="6">
@@ -1661,10 +1657,10 @@
       <c r="A33" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="5">
+      <c r="B33" s="11">
         <v>1.3966670000000001E-3</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="12">
         <v>1.5904999999999999E-3</v>
       </c>
       <c r="D33" s="6">
@@ -1676,10 +1672,10 @@
       <c r="A34" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B34" s="11">
         <v>4.5049741670000003</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C34" s="12">
         <v>5.6573946670000002</v>
       </c>
       <c r="D34" s="6">
@@ -1691,10 +1687,10 @@
       <c r="A35" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B35" s="11">
         <v>3.1722638330000001</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C35" s="12">
         <v>4.3632534999999999</v>
       </c>
       <c r="D35" s="6">
@@ -1702,17 +1698,17 @@
         <v>1.3754384028877209</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="16" thickBot="1">
-      <c r="A36" s="7" t="s">
+    <row r="36" spans="1:4">
+      <c r="A36" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B36" s="7">
+      <c r="B36" s="11">
         <v>5.1898141669999998</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="12">
         <v>7.8649428329999997</v>
       </c>
-      <c r="D36" s="8">
+      <c r="D36" s="6">
         <f t="shared" si="0"/>
         <v>1.5154575057831738</v>
       </c>
@@ -1729,7 +1725,6 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" scale="66" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>